<commit_message>
update: (2023-03-21) perbaikan dan penambahan code
</commit_message>
<xml_diff>
--- a/src/public/excel/Template Data Siswa.xlsx
+++ b/src/public/excel/Template Data Siswa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85423484-8A6A-4C8E-9F13-4C261606DE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E99576-9D7D-4687-8872-21407D681922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
   <si>
     <t>NAMA</t>
   </si>
@@ -506,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -514,7 +514,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1027,7 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1135,9 +1134,6 @@
       </c>
       <c r="AK2" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>60</v>

</xml_diff>